<commit_message>
update write add props/vars
</commit_message>
<xml_diff>
--- a/spreadsheet.xlsx
+++ b/spreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Matthias Gültig\Documents\pyThermoML\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70EF566F-C029-4C06-BADE-7DF120030AFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{853A1595-54BD-453F-8459-BA4E6B96FAAD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{059A8766-B3CA-40C2-821B-F4DEE17D28FE}"/>
+    <workbookView xWindow="15870" yWindow="4530" windowWidth="18000" windowHeight="9360" xr2:uid="{059A8766-B3CA-40C2-821B-F4DEE17D28FE}"/>
   </bookViews>
   <sheets>
     <sheet name="Spreadsheet" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="29">
   <si>
     <t>Title</t>
   </si>
@@ -100,9 +100,6 @@
     <t>CompoundID</t>
   </si>
   <si>
-    <t>InChiCode</t>
-  </si>
-  <si>
     <t>CommonName</t>
   </si>
   <si>
@@ -113,6 +110,18 @@
   </si>
   <si>
     <t>Datapoint</t>
+  </si>
+  <si>
+    <t>InchiCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Examination of … </t>
+  </si>
+  <si>
+    <t>DOI8444</t>
+  </si>
+  <si>
+    <t>Author1, Author2</t>
   </si>
 </sst>
 </file>
@@ -258,21 +267,21 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -648,7 +657,7 @@
   <dimension ref="A1:R37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G22" sqref="G22"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -662,15 +671,15 @@
     <col min="8" max="8" width="14.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A1" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="15"/>
-    </row>
-    <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="16"/>
-      <c r="B2" s="17"/>
+    <row r="1" spans="1:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="16" t="s">
+        <v>22</v>
+      </c>
+      <c r="B1" s="17"/>
+    </row>
+    <row r="2" spans="1:8" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="18"/>
+      <c r="B2" s="19"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
@@ -687,11 +696,17 @@
     </row>
     <row r="6" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C6" s="11" t="s">
-        <v>24</v>
-      </c>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="10"/>
+        <v>23</v>
+      </c>
+      <c r="D6" s="9" t="s">
+        <v>26</v>
+      </c>
+      <c r="E6" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="F6" s="10" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="9" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
@@ -700,7 +715,7 @@
         <v>20</v>
       </c>
       <c r="E10" s="3" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="F10" s="3" t="s">
         <v>3</v>
@@ -709,7 +724,7 @@
         <v>4</v>
       </c>
       <c r="H10" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
@@ -721,7 +736,7 @@
       </c>
       <c r="E11" s="5"/>
       <c r="F11" s="5"/>
-      <c r="G11" s="18"/>
+      <c r="G11" s="14"/>
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
@@ -811,20 +826,18 @@
     </row>
     <row r="20" spans="2:18" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21" spans="2:18" x14ac:dyDescent="0.25">
       <c r="C21" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="D21" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3" t="str">
         <f>IF(ISBLANK($D$23), "","other property" )</f>
-        <v>other property</v>
+        <v/>
       </c>
       <c r="G21" s="3"/>
       <c r="H21" s="3"/>
@@ -852,7 +865,7 @@
       </c>
       <c r="D22" s="5" t="str">
         <f>IF(D21="viscosity","Pa s",IF(D21="peakTemperature","K",IF(D21="massDensity","kg/m3",IF(D21="microviscosity","Pa s",""))))</f>
-        <v>Pa s</v>
+        <v/>
       </c>
       <c r="E22" s="5"/>
       <c r="F22" s="5"/>
@@ -909,9 +922,7 @@
       <c r="C23" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="D23" s="19">
-        <v>1</v>
-      </c>
+      <c r="D23" s="15"/>
       <c r="E23" s="5"/>
       <c r="F23" s="5"/>
       <c r="G23" s="5"/>
@@ -925,7 +936,7 @@
       <c r="O23" s="5"/>
       <c r="P23" s="6"/>
     </row>
-    <row r="24" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:18" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C24" s="7"/>
       <c r="D24" s="5"/>
       <c r="E24" s="5"/>
@@ -941,7 +952,7 @@
       <c r="O24" s="5"/>
       <c r="P24" s="6"/>
     </row>
-    <row r="25" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:18" hidden="1" x14ac:dyDescent="0.25">
       <c r="C25" s="7"/>
       <c r="D25" s="5"/>
       <c r="E25" s="5"/>
@@ -957,7 +968,7 @@
       <c r="O25" s="5"/>
       <c r="P25" s="6"/>
     </row>
-    <row r="26" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:18" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C26" s="7"/>
       <c r="D26" s="5"/>
       <c r="E26" s="5"/>
@@ -973,7 +984,7 @@
       <c r="O26" s="5"/>
       <c r="P26" s="6"/>
     </row>
-    <row r="27" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:18" ht="2.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C27" s="7"/>
       <c r="D27" s="5"/>
       <c r="E27" s="5"/>
@@ -989,7 +1000,7 @@
       <c r="O27" s="5"/>
       <c r="P27" s="6"/>
     </row>
-    <row r="28" spans="2:18" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:18" ht="1.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="C28" s="7"/>
       <c r="D28" s="5"/>
       <c r="E28" s="5"/>
@@ -1040,7 +1051,7 @@
       <c r="E30" s="5"/>
       <c r="F30" s="5"/>
       <c r="G30" s="5" t="str">
-        <f t="shared" ref="E30:P30" si="1">IF(G29="moleFraction","-",IF(G29="temperature","K",IF(G29="upperTemperature","K",IF(G29="lowerTemperature","K",""))))</f>
+        <f t="shared" ref="G30:P30" si="1">IF(G29="moleFraction","-",IF(G29="temperature","K",IF(G29="upperTemperature","K",IF(G29="lowerTemperature","K",""))))</f>
         <v/>
       </c>
       <c r="H30" s="5"/>
@@ -1103,9 +1114,6 @@
       <c r="B37" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="A1:B2"/>
-  </mergeCells>
   <dataValidations count="3">
     <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="D21 P21 G21 J21 M21" xr:uid="{82FC33DB-7443-4D3F-A43E-22EBE1405FE4}">
       <formula1>INDIRECT("grid_prop[Properties]")</formula1>

</xml_diff>